<commit_message>
Actualización 13 de mayo de 2024 - Lap HP
Se actualiza el repositorio con el material del curso.
</commit_message>
<xml_diff>
--- a/Bitacoras/Parcial_03/Bitacora_Laboratorio_Fisica_IV_NRC_95_Parcial_03.xlsx
+++ b/Bitacoras/Parcial_03/Bitacora_Laboratorio_Fisica_IV_NRC_95_Parcial_03.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_4\Bitacoras\Parcial_03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C2DBD4-A5ED-479E-9DEF-89D65B6D4F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A338BEBB-6098-421C-B852-F34D5BE6D829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="840" xr2:uid="{5A885302-ACD9-4B6A-A6FB-2597D2976EB6}"/>
   </bookViews>
@@ -682,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AFA2C3-0AB5-4100-B988-15F96676F5E9}">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +701,7 @@
     <col min="18" max="18" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -756,8 +756,11 @@
       <c r="R1" s="5">
         <v>45384</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" s="6">
+        <v>45391</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>80178045</v>
       </c>
@@ -783,8 +786,11 @@
       <c r="Q2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>20197413</v>
       </c>
@@ -811,7 +817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>20270657</v>
       </c>
@@ -835,7 +841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>80204265</v>
       </c>
@@ -868,7 +874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>20228454</v>
       </c>
@@ -895,7 +901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>20194829</v>
       </c>
@@ -919,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>20195555</v>
       </c>
@@ -940,7 +946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>20198334</v>
       </c>
@@ -966,8 +972,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>10188042</v>
       </c>
@@ -997,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>80209587</v>
       </c>
@@ -1021,7 +1030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10185845</v>
       </c>
@@ -1042,7 +1051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>20184819</v>
       </c>

</xml_diff>